<commit_message>
fix bugs in itemgap excel
</commit_message>
<xml_diff>
--- a/media/gap_report.xlsx
+++ b/media/gap_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,67 +436,167 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>Facility id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Facility name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>code</t>
+          <t>Facility code</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>level</t>
+          <t>Level name</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>parent</t>
+          <t xml:space="preserve">parent Facility </t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>general</t>
+          <t>general population</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>children</t>
+          <t>under 1 population</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>Facility type</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>tcapacity1</t>
+          <t>Total capacity for +2 to +8</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>fcapacity1</t>
+          <t>Functioning capacity for +2 to +8</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>req1</t>
+          <t>Required capacity for +2 to +8</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>excees1</t>
+          <t>Diffrence between required capacity and available +2 to +8</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>exceed1</t>
+          <t>Excess +2 - +8C</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total capacity for + -20C </t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Functioning capacity for + -20C </t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Required capacity for + -20C </t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Diffrence between required capacity and available + -20C</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Excess -20C</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Total capacity for -70 C</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Functioning capacity for -70 C</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Required capacity for -70 C</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Diffrence between required capacity and available -70 C</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Excess -70C</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Total capacity for +25C</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Functioning capacity for +25C</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Required capacity for +25C</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Diffrence between required capacity and available +25C</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Excess +25C</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Total capacity for Dry store</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Functioning capacity for Dry store</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Required capacity for Dry store</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Diffrence between required capacity and available Dry store</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Excess Dry store</t>
         </is>
       </c>
     </row>
@@ -505,31 +605,39 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>central store</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>test4</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>abc0200013</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>sa</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>850</v>
+      </c>
+      <c r="H2" t="n">
+        <v>500</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>--</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>200</v>
-      </c>
-      <c r="H2" t="n">
-        <v>250</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
         <v>0</v>
       </c>
@@ -546,8 +654,94 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="N2" t="b">
-        <v>0</v>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -555,31 +749,39 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>test4</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>abc0200013</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>test1</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>central store</t>
-        </is>
-      </c>
       <c r="G3" t="n">
-        <v>750</v>
+        <v>850</v>
       </c>
       <c r="H3" t="n">
-        <v>700</v>
-      </c>
-      <c r="I3" t="inlineStr"/>
+        <v>500</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
@@ -596,8 +798,94 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="N3" t="b">
-        <v>0</v>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AD3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -605,17 +893,21 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>test2</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>test4</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>abc0200013</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>sdadads</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -624,12 +916,16 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>150</v>
+        <v>850</v>
       </c>
       <c r="H4" t="n">
-        <v>100</v>
-      </c>
-      <c r="I4" t="inlineStr"/>
+        <v>500</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
@@ -646,8 +942,94 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="N4" t="b">
-        <v>0</v>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -655,31 +1037,39 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>test3</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>test4</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>abc0200013</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>asdad</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>400</v>
+        <v>850</v>
       </c>
       <c r="H5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
+        <v>500</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
@@ -696,8 +1086,94 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="N5" t="b">
-        <v>0</v>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -705,14 +1181,18 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>test4</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>abc0200013</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>0</t>
@@ -720,16 +1200,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>test3</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>600</v>
+        <v>850</v>
       </c>
       <c r="H6" t="n">
-        <v>600</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
+        <v>500</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
       <c r="J6" t="n">
         <v>0</v>
       </c>
@@ -746,8 +1230,94 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="N6" t="b">
-        <v>0</v>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -783,7 +1353,11 @@
       <c r="H7" t="n">
         <v>500</v>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
@@ -800,8 +1374,94 @@
           <t>0.00</t>
         </is>
       </c>
-      <c r="N7" t="b">
-        <v>0</v>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bugs in gap map
</commit_message>
<xml_diff>
--- a/media/gap_report.xlsx
+++ b/media/gap_report.xlsx
@@ -496,7 +496,7 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Excess +2 - +8C</t>
+          <t>Excess +2 to +8</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
@@ -605,33 +605,29 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>test4</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>abc0200013</t>
-        </is>
-      </c>
+          <t>central store</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>sa</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>--</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>850</v>
+        <v>200</v>
       </c>
       <c r="H2" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -749,18 +745,14 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>test4</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>abc0200013</t>
-        </is>
-      </c>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>0</t>
@@ -768,14 +760,14 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>central store</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="H3" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -893,21 +885,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>test4</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>abc0200013</t>
-        </is>
-      </c>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>sdadads</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -916,10 +904,10 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>850</v>
+        <v>150</v>
       </c>
       <c r="H4" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -1037,33 +1025,29 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>test4</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>abc0200013</t>
-        </is>
-      </c>
+          <t>test3</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>asdad</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>850</v>
+        <v>400</v>
       </c>
       <c r="H5" t="n">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -1181,18 +1165,14 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>test4</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>abc0200013</t>
-        </is>
-      </c>
+          <t>mamad</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>0</t>
@@ -1200,14 +1180,14 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>test3</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>850</v>
+        <v>600</v>
       </c>
       <c r="H6" t="n">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
change gap item view for new report
</commit_message>
<xml_diff>
--- a/media/gap_report.xlsx
+++ b/media/gap_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,106 +499,6 @@
           <t>Excess +2 to +8</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Total capacity for + -20C </t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Functioning capacity for + -20C </t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Required capacity for + -20C </t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Diffrence between required capacity and available + -20C</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Excess -20C</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Total capacity for -70 C</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Functioning capacity for -70 C</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Required capacity for -70 C</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Diffrence between required capacity and available -70 C</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Excess -70C</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Total capacity for +25C</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Functioning capacity for +25C</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Required capacity for +25C</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Diffrence between required capacity and available +25C</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Excess +25C</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Total capacity for Dry store</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>Functioning capacity for Dry store</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>Required capacity for Dry store</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>Diffrence between required capacity and available Dry store</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>Excess Dry store</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -651,90 +551,6 @@
         </is>
       </c>
       <c r="N2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="T2" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0</v>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="Y2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
         <is>
           <t>False</t>
         </is>
@@ -795,90 +611,6 @@
           <t>False</t>
         </is>
       </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="T3" t="n">
-        <v>0</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="Y3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="AD3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -935,90 +667,6 @@
           <t>False</t>
         </is>
       </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="T4" t="n">
-        <v>0</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="AD4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1075,90 +723,6 @@
           <t>False</t>
         </is>
       </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1215,90 +779,6 @@
           <t>False</t>
         </is>
       </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1355,90 +835,6 @@
         </is>
       </c>
       <c r="N7" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="T7" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="Y7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>

<commit_message>
alter owner field on user
</commit_message>
<xml_diff>
--- a/media/gap_report.xlsx
+++ b/media/gap_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,17 +505,21 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>central store</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>Innovasiya və Təchizat Mərkəzi</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>AZE0100001</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>sa</t>
+          <t>Central</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -524,10 +528,10 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>200</v>
+        <v>10200000</v>
       </c>
       <c r="H2" t="n">
-        <v>250</v>
+        <v>300000</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -535,308 +539,20 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1010484</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="L2" t="n">
+        <v>308550</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-308550</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>9</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>test1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>central store</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>750</v>
-      </c>
-      <c r="H3" t="n">
-        <v>700</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>test2</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>sdadads</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>test1</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>150</v>
-      </c>
-      <c r="H4" t="n">
-        <v>100</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>11</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>test3</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>asdad</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>test2</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>400</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1200</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>12</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>mamad</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>test3</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>600</v>
-      </c>
-      <c r="H6" t="n">
-        <v>600</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>13</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>test4</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>abc0200013</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>test1</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>850</v>
-      </c>
-      <c r="H7" t="n">
-        <v>500</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
     </row>

</xml_diff>